<commit_message>
Edited the Gantt Chart
</commit_message>
<xml_diff>
--- a/KTANE Gantt.xlsx
+++ b/KTANE Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff19d073d2d85eb6/Documents/Text Docs/Uni/Freshman/Spring 2021/CSC 132/mygitfolder/CSC-Final-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12253\Documents\CSC Files\CSC 132\CSC-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{F165FD7E-15F7-4EC4-A6AE-4BEB855BC866}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1C5029FA-39A8-4D87-BDEA-4491A2D63482}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C176D12-800E-4C43-B030-CDA816C0697E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4792406-7784-49BF-B9AB-10C18735CF3F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{D4792406-7784-49BF-B9AB-10C18735CF3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,50 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>GUI</t>
   </si>
   <si>
-    <t>Module 1</t>
-  </si>
-  <si>
-    <t>Module 2</t>
-  </si>
-  <si>
-    <t>Module 3</t>
-  </si>
-  <si>
-    <t>Module 4</t>
-  </si>
-  <si>
-    <t>Module 5</t>
-  </si>
-  <si>
-    <t>Module 6</t>
-  </si>
-  <si>
     <t>General Module "Skeleton" Class</t>
   </si>
   <si>
@@ -97,13 +58,61 @@
   </si>
   <si>
     <t>Final Touch-Ups</t>
+  </si>
+  <si>
+    <t>Final Presentation</t>
+  </si>
+  <si>
+    <t>Week1: 3/28 - 4/3</t>
+  </si>
+  <si>
+    <t>Week2: 4/4 - 4/10</t>
+  </si>
+  <si>
+    <t>Week3: 4/11 - 4/17</t>
+  </si>
+  <si>
+    <t>Week4: 4/18 - 4/24</t>
+  </si>
+  <si>
+    <t>Week5: 4/25 - 5/1</t>
+  </si>
+  <si>
+    <t>Week6: 5/2 - 5/8</t>
+  </si>
+  <si>
+    <t>Week7: 5/9 - 5/15</t>
+  </si>
+  <si>
+    <t>Module 3: "Simon Says"</t>
+  </si>
+  <si>
+    <t>Module 1: "The Wires"</t>
+  </si>
+  <si>
+    <t>Module 5: "The Button"</t>
+  </si>
+  <si>
+    <t>Module 6: "Keypads"</t>
+  </si>
+  <si>
+    <t>Module 4: "Memory"</t>
+  </si>
+  <si>
+    <t>Module 2: "Morse Code"</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="[$-409]ddd\,\ mmm\ d"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +126,21 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +171,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -158,20 +204,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
+    <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,129 +569,871 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5144F41D-2708-4B05-8EB3-151814EC805B}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:AX19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="A1:H15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="35" style="1" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.89453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.89453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.62890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.89453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.05078125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.05078125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.1015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.62890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.3671875" style="1" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.9453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+    </row>
+    <row r="2" spans="1:50" s="12" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="11"/>
+      <c r="B2" s="13">
+        <v>44283</v>
+      </c>
+      <c r="C2" s="13">
+        <v>44284</v>
+      </c>
+      <c r="D2" s="13">
+        <v>44285</v>
+      </c>
+      <c r="E2" s="13">
+        <v>44286</v>
+      </c>
+      <c r="F2" s="13">
+        <v>44287</v>
+      </c>
+      <c r="G2" s="13">
+        <v>44288</v>
+      </c>
+      <c r="H2" s="13">
+        <v>44289</v>
+      </c>
+      <c r="I2" s="13">
+        <v>44290</v>
+      </c>
+      <c r="J2" s="13">
+        <v>44291</v>
+      </c>
+      <c r="K2" s="13">
+        <v>44292</v>
+      </c>
+      <c r="L2" s="13">
+        <v>44293</v>
+      </c>
+      <c r="M2" s="13">
+        <v>44294</v>
+      </c>
+      <c r="N2" s="13">
+        <v>44295</v>
+      </c>
+      <c r="O2" s="13">
+        <v>44296</v>
+      </c>
+      <c r="P2" s="13">
+        <v>44297</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>44298</v>
+      </c>
+      <c r="R2" s="13">
+        <v>44299</v>
+      </c>
+      <c r="S2" s="13">
+        <v>44300</v>
+      </c>
+      <c r="T2" s="13">
+        <v>44301</v>
+      </c>
+      <c r="U2" s="13">
+        <v>44302</v>
+      </c>
+      <c r="V2" s="13">
+        <v>44303</v>
+      </c>
+      <c r="W2" s="13">
+        <v>44304</v>
+      </c>
+      <c r="X2" s="13">
+        <v>44305</v>
+      </c>
+      <c r="Y2" s="13">
+        <v>44306</v>
+      </c>
+      <c r="Z2" s="13">
+        <v>44307</v>
+      </c>
+      <c r="AA2" s="13">
+        <v>44308</v>
+      </c>
+      <c r="AB2" s="13">
+        <v>44309</v>
+      </c>
+      <c r="AC2" s="13">
+        <v>44310</v>
+      </c>
+      <c r="AD2" s="13">
+        <v>44311</v>
+      </c>
+      <c r="AE2" s="13">
+        <v>44312</v>
+      </c>
+      <c r="AF2" s="13">
+        <v>44313</v>
+      </c>
+      <c r="AG2" s="13">
+        <v>44314</v>
+      </c>
+      <c r="AH2" s="13">
+        <v>44315</v>
+      </c>
+      <c r="AI2" s="13">
+        <v>44316</v>
+      </c>
+      <c r="AJ2" s="13">
+        <v>44317</v>
+      </c>
+      <c r="AK2" s="13">
+        <v>44318</v>
+      </c>
+      <c r="AL2" s="13">
+        <v>44319</v>
+      </c>
+      <c r="AM2" s="13">
+        <v>44320</v>
+      </c>
+      <c r="AN2" s="13">
+        <v>44321</v>
+      </c>
+      <c r="AO2" s="13">
+        <v>44322</v>
+      </c>
+      <c r="AP2" s="13">
+        <v>44323</v>
+      </c>
+      <c r="AQ2" s="13">
+        <v>44324</v>
+      </c>
+      <c r="AR2" s="13">
+        <v>44325</v>
+      </c>
+      <c r="AS2" s="13">
+        <v>44326</v>
+      </c>
+      <c r="AT2" s="13">
+        <v>44327</v>
+      </c>
+      <c r="AU2" s="13">
+        <v>44328</v>
+      </c>
+      <c r="AV2" s="13">
+        <v>44329</v>
+      </c>
+      <c r="AW2" s="13">
+        <v>44330</v>
+      </c>
+      <c r="AX2" s="13">
+        <v>44331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="3"/>
+    </row>
+    <row r="4" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="3"/>
+    </row>
+    <row r="5" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AV5" s="3"/>
+      <c r="AW5" s="3"/>
+      <c r="AX5" s="3"/>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="3"/>
+      <c r="AX6" s="3"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
+      <c r="AX7" s="3"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="3"/>
+      <c r="AW8" s="3"/>
+      <c r="AX8" s="3"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+      <c r="AU9" s="3"/>
+      <c r="AV9" s="3"/>
+      <c r="AW9" s="3"/>
+      <c r="AX9" s="3"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+      <c r="AU10" s="3"/>
+      <c r="AV10" s="3"/>
+      <c r="AW10" s="3"/>
+      <c r="AX10" s="3"/>
+    </row>
+    <row r="11" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+      <c r="AU11" s="3"/>
+      <c r="AV11" s="3"/>
+      <c r="AW11" s="3"/>
+      <c r="AX11" s="3"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="15"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="15"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+      <c r="AU12" s="14"/>
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="3"/>
+      <c r="AX12" s="3"/>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.5">
+      <c r="A16" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A17" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A18" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="AR1:AX1"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AC1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changed my preferred modules
</commit_message>
<xml_diff>
--- a/KTANE Gantt.xlsx
+++ b/KTANE Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12253\Documents\CSC Files\CSC 132\CSC-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff19d073d2d85eb6/Documents/Text Docs/Uni/Freshman/Spring 2021/CSC 132/mygitfolder/CSC-Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C176D12-800E-4C43-B030-CDA816C0697E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3C176D12-800E-4C43-B030-CDA816C0697E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EC6B5ADC-4250-49A7-9EAD-48634924169B}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{D4792406-7784-49BF-B9AB-10C18735CF3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4792406-7784-49BF-B9AB-10C18735CF3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>GUI</t>
   </si>
@@ -99,10 +99,7 @@
     <t>Module 4: "Memory"</t>
   </si>
   <si>
-    <t>Module 2: "Morse Code"</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>Module 2: "Ultrasonic"</t>
   </si>
 </sst>
 </file>
@@ -110,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]ddd\,\ mmm\ d"/>
+    <numFmt numFmtId="164" formatCode="[$-409]ddd\,\ mmm\ d"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -238,16 +235,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
@@ -569,290 +566,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5144F41D-2708-4B05-8EB3-151814EC805B}">
-  <dimension ref="A1:AX19"/>
+  <dimension ref="A1:AX18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.89453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.89453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.62890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.3671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.89453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.05078125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.05078125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.20703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.20703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.1015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.3671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.62890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.3671875" style="1" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="10.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.20703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.20703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="16384" width="9.15625" style="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10" t="s">
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10" t="s">
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-    </row>
-    <row r="2" spans="1:50" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="11"/>
-      <c r="B2" s="13">
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+    </row>
+    <row r="2" spans="1:50" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="12">
         <v>44283</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>44284</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>44285</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>44286</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>44287</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>44288</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>44289</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <v>44290</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <v>44291</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="12">
         <v>44292</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="12">
         <v>44293</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="12">
         <v>44294</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <v>44295</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="12">
         <v>44296</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="12">
         <v>44297</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="12">
         <v>44298</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="12">
         <v>44299</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="12">
         <v>44300</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="12">
         <v>44301</v>
       </c>
-      <c r="U2" s="13">
+      <c r="U2" s="12">
         <v>44302</v>
       </c>
-      <c r="V2" s="13">
+      <c r="V2" s="12">
         <v>44303</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="12">
         <v>44304</v>
       </c>
-      <c r="X2" s="13">
+      <c r="X2" s="12">
         <v>44305</v>
       </c>
-      <c r="Y2" s="13">
+      <c r="Y2" s="12">
         <v>44306</v>
       </c>
-      <c r="Z2" s="13">
+      <c r="Z2" s="12">
         <v>44307</v>
       </c>
-      <c r="AA2" s="13">
+      <c r="AA2" s="12">
         <v>44308</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="AB2" s="12">
         <v>44309</v>
       </c>
-      <c r="AC2" s="13">
+      <c r="AC2" s="12">
         <v>44310</v>
       </c>
-      <c r="AD2" s="13">
+      <c r="AD2" s="12">
         <v>44311</v>
       </c>
-      <c r="AE2" s="13">
+      <c r="AE2" s="12">
         <v>44312</v>
       </c>
-      <c r="AF2" s="13">
+      <c r="AF2" s="12">
         <v>44313</v>
       </c>
-      <c r="AG2" s="13">
+      <c r="AG2" s="12">
         <v>44314</v>
       </c>
-      <c r="AH2" s="13">
+      <c r="AH2" s="12">
         <v>44315</v>
       </c>
-      <c r="AI2" s="13">
+      <c r="AI2" s="12">
         <v>44316</v>
       </c>
-      <c r="AJ2" s="13">
+      <c r="AJ2" s="12">
         <v>44317</v>
       </c>
-      <c r="AK2" s="13">
+      <c r="AK2" s="12">
         <v>44318</v>
       </c>
-      <c r="AL2" s="13">
+      <c r="AL2" s="12">
         <v>44319</v>
       </c>
-      <c r="AM2" s="13">
+      <c r="AM2" s="12">
         <v>44320</v>
       </c>
-      <c r="AN2" s="13">
+      <c r="AN2" s="12">
         <v>44321</v>
       </c>
-      <c r="AO2" s="13">
+      <c r="AO2" s="12">
         <v>44322</v>
       </c>
-      <c r="AP2" s="13">
+      <c r="AP2" s="12">
         <v>44323</v>
       </c>
-      <c r="AQ2" s="13">
+      <c r="AQ2" s="12">
         <v>44324</v>
       </c>
-      <c r="AR2" s="13">
+      <c r="AR2" s="12">
         <v>44325</v>
       </c>
-      <c r="AS2" s="13">
+      <c r="AS2" s="12">
         <v>44326</v>
       </c>
-      <c r="AT2" s="13">
+      <c r="AT2" s="12">
         <v>44327</v>
       </c>
-      <c r="AU2" s="13">
+      <c r="AU2" s="12">
         <v>44328</v>
       </c>
-      <c r="AV2" s="13">
+      <c r="AV2" s="12">
         <v>44329</v>
       </c>
-      <c r="AW2" s="13">
+      <c r="AW2" s="12">
         <v>44330</v>
       </c>
-      <c r="AX2" s="13">
+      <c r="AX2" s="12">
         <v>44331</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:50" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -906,7 +902,7 @@
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
     </row>
-    <row r="4" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -960,7 +956,7 @@
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
     </row>
-    <row r="5" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1010,7 @@
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1068,7 +1064,7 @@
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1122,7 +1118,7 @@
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1176,7 +1172,7 @@
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1230,7 +1226,7 @@
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1284,7 +1280,7 @@
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
     </row>
-    <row r="11" spans="1:50" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1338,7 +1334,7 @@
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1373,54 +1369,49 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
-      <c r="AG12" s="15"/>
+      <c r="AG12" s="14"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
       <c r="AM12" s="3"/>
-      <c r="AN12" s="15"/>
+      <c r="AN12" s="14"/>
       <c r="AO12" s="3"/>
       <c r="AP12" s="3"/>
       <c r="AQ12" s="3"/>
       <c r="AR12" s="3"/>
       <c r="AS12" s="3"/>
       <c r="AT12" s="3"/>
-      <c r="AU12" s="14"/>
+      <c r="AU12" s="13"/>
       <c r="AV12" s="3"/>
       <c r="AW12" s="3"/>
       <c r="AX12" s="3"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="I19" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>